<commit_message>
Update info in the documentation.xlsx
</commit_message>
<xml_diff>
--- a/documentation.xlsx
+++ b/documentation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haqim\Desktop\personal\interview11062022\files to github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haqim\Desktop\for github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D993283B-B76C-404A-A478-2C6FA037CA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4CF5F7-6918-44FD-BEA1-2FAFE07099C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{13C12EFE-B736-4833-9B08-03ACBC860603}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{13C12EFE-B736-4833-9B08-03ACBC860603}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction for running" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
   <si>
     <t>produces</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>2. After click "Sign in with Google", we will directed to this page. We can start Sign In to Google.</t>
+  </si>
+  <si>
+    <t>Please add it to the code at : server side\googleSignInConfig.php</t>
   </si>
 </sst>
 </file>
@@ -3000,7 +3003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB025277-4B62-42AE-BA15-80074CFDA552}">
   <dimension ref="F10:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C7" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -3238,10 +3241,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B298CC97-231C-4C0A-8360-468EEE6A49D9}">
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3307,25 +3310,14 @@
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
       <c r="K9" s="7"/>
-      <c r="L9" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -3336,13 +3328,13 @@
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="7"/>
-      <c r="M10" t="s">
-        <v>49</v>
+      <c r="L10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -3354,14 +3346,14 @@
       <c r="J11" s="9"/>
       <c r="K11" s="7"/>
       <c r="M11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="B12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -3371,13 +3363,13 @@
       <c r="J12" s="9"/>
       <c r="K12" s="7"/>
       <c r="M12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" s="9"/>
       <c r="C13" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -3387,11 +3379,14 @@
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="7"/>
+      <c r="M13" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" s="9"/>
       <c r="C14" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -3401,103 +3396,99 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="7"/>
-      <c r="L14" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
       <c r="K15" s="7"/>
       <c r="L15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K16" s="7"/>
+      <c r="L16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>4</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="K16" s="7"/>
-      <c r="M16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="K17" s="7"/>
       <c r="M17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K18" s="7"/>
+      <c r="M18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>5</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>41</v>
       </c>
-      <c r="K18" s="7"/>
-      <c r="M18" s="9" t="s">
+      <c r="K19" s="7"/>
+      <c r="M19" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K19" s="7"/>
-      <c r="M19" t="s">
-        <v>57</v>
-      </c>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K20" s="7"/>
-      <c r="N20" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
+      <c r="M20" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="K21" s="7"/>
+      <c r="N21" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
         <v>43</v>
       </c>
-      <c r="K21" s="7"/>
-      <c r="M21" t="s">
+      <c r="K22" s="7"/>
+      <c r="M22" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B22" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="10"/>
-      <c r="N22" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="O22" s="11"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -3508,27 +3499,42 @@
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="10"/>
-      <c r="M23" s="9" t="s">
+      <c r="N23" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="O23" s="11"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B24" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="10"/>
+      <c r="M24" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="K24" s="7"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" s="6">
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
         <v>6</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="K25" s="7"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="K26" s="7"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
@@ -3538,7 +3544,7 @@
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="K29" s="8"/>
+      <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="K30" s="8"/>
@@ -3569,6 +3575,9 @@
     </row>
     <row r="39" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K39" s="8"/>
+    </row>
+    <row r="40" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K40" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add "Running with Docker" section
</commit_message>
<xml_diff>
--- a/documentation.xlsx
+++ b/documentation.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haqim\Desktop\for github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haqim\Desktop\docker\docker files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4CF5F7-6918-44FD-BEA1-2FAFE07099C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1CE044-8827-44CB-AA20-0BA4B21EF076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{13C12EFE-B736-4833-9B08-03ACBC860603}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{13C12EFE-B736-4833-9B08-03ACBC860603}"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction for running" sheetId="2" r:id="rId1"/>
     <sheet name="Instruction for testing" sheetId="3" r:id="rId2"/>
     <sheet name="Instruction for building" sheetId="4" r:id="rId3"/>
     <sheet name="Interface documentation" sheetId="5" r:id="rId4"/>
+    <sheet name="Running with docker" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="132">
   <si>
     <t>produces</t>
   </si>
@@ -290,13 +291,157 @@
   </si>
   <si>
     <t>Please add it to the code at : server side\googleSignInConfig.php</t>
+  </si>
+  <si>
+    <t>2. Extract the content of the zip file</t>
+  </si>
+  <si>
+    <t>3. Insert your client id and secret id by following this step:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> docker build -t ubuntu_gcc_libcurl .</t>
+  </si>
+  <si>
+    <t>a.</t>
+  </si>
+  <si>
+    <t>Please put your redirect URL as follow:</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/myWampVirtualHost/googleSignIn/createUserIdWithGoogleAcc.php</t>
+  </si>
+  <si>
+    <t>[Note: please change the "localhost" into your IP address in case you access using you container IP]</t>
+  </si>
+  <si>
+    <t>c. Open powershell, and insert command as below to setup the docker for server side.</t>
+  </si>
+  <si>
+    <t>b. docker-compose up</t>
+  </si>
+  <si>
+    <t>d. You can start sign in to using your google account by going to the below url</t>
+  </si>
+  <si>
+    <t>1. Download the file called "Docker files 21062022.zip" from github</t>
+  </si>
+  <si>
+    <t>a. cd /path/to/"docker file 21062022"/"server side"</t>
+  </si>
+  <si>
+    <t>b. Go to "server side\php\src\myWampVirtualHost\googleSignIn\googleSignInConfig.php" and fill in your client id and secret id in the line below:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a. docker-compose build   </t>
+  </si>
+  <si>
+    <t>[Note: please follow the "Interface documentation" for the next step</t>
+  </si>
+  <si>
+    <t>Please note that, in this docker environment (Debian), the fwrite() seems like not functioning.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The file toDoListUserId.txt is generated, but no value in it. </t>
+  </si>
+  <si>
+    <t>Server side</t>
+  </si>
+  <si>
+    <t>It is suspected that this issue is related to file permission. Please copy the userId (highlighted with yellow color) for later use in the client side]</t>
+  </si>
+  <si>
+    <t>Client side</t>
+  </si>
+  <si>
+    <t>1. Go to "\path\to\Docker files 2106202\client side\client side"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. [OPTIONAL STEP] Modify the part with yellow highlight in case your container have different IP </t>
+  </si>
+  <si>
+    <t>and you want to test it directly without inputting any url value when presssing "3".</t>
+  </si>
+  <si>
+    <t>4. Using Powershell,  go to "\path\to\Docker files 2106202\client side" . This is where the "Dockerfile" situated</t>
+  </si>
+  <si>
+    <t>5. Eexecute the command as below:</t>
+  </si>
+  <si>
+    <t>6. After it has finish, go to Docker Desktop -&gt; Images . Then, run the ubuntu_gcc_libcurl image</t>
+  </si>
+  <si>
+    <t>In my case, I put the container name as "ubuntu_gcc_libcurl"</t>
+  </si>
+  <si>
+    <t>7. Then go to Docker Desktop -&gt; Container. Find the container "ubuntu_gcc_libcurl" and run. After that, open the terminal.</t>
+  </si>
+  <si>
+    <t>[Note: yaml file for docker-compose can be obtained at inside "server side" folder, while Dockerfile can be</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> obtained at  "server side/php"]</t>
+  </si>
+  <si>
+    <t>8. Inside the "ubuntu_gcc_libcurl" container terminal, do the following commands:</t>
+  </si>
+  <si>
+    <t>2. Modify the userId in toDoListUserId.txt with your userId generated from server side. Currently, it has been set as user1</t>
+  </si>
+  <si>
+    <t>a. cd client_side</t>
+  </si>
+  <si>
+    <t>b. to test libcurl is working, do the following:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         g++ test_for_curl.cpp -lcurl -o test_for_curl.exe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         ./test_for_curl.exe</t>
+  </si>
+  <si>
+    <t>you will get the output as below. This mean the libcurl is working</t>
+  </si>
+  <si>
+    <t>c. you can start running the todolist cpp file. To run, do the following:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        g++ class_test.cpp OperationRequest.cpp -lcurl -o class_test.exe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ./class_test.exe</t>
+  </si>
+  <si>
+    <t>you will get output as shown in the sheet called "Interface documentation"</t>
+  </si>
+  <si>
+    <t>However, during my checking using the container, we will get the output as below when</t>
+  </si>
+  <si>
+    <t>The output "curl_easy_perform() faild: couldn’t connect to server" occur here because</t>
+  </si>
+  <si>
+    <t>the my current container's network does not setup/linked properly to the localhost.</t>
+  </si>
+  <si>
+    <t>we are trying to perform POST request to the server. Since we are able to</t>
+  </si>
+  <si>
+    <t>get reply from example.com during checking using test_for_curl.cpp, this mean the program</t>
+  </si>
+  <si>
+    <t>is still working correctly, but it cannot perform the connection to localhost because</t>
+  </si>
+  <si>
+    <t>the network is not being setup properly.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,6 +460,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -340,7 +492,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -357,11 +509,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -380,6 +541,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2699,6 +2863,372 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>503452</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>175510</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92FBE820-1FB9-0C07-8FBC-3C821D3B5844}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1066800" y="2049780"/>
+          <a:ext cx="6142252" cy="2880610"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACE31C22-ADCC-A7D8-22CB-4BC1A2511B00}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4130040" y="3985260"/>
+          <a:ext cx="1539240" cy="1112520"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>404518</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>160138</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AAD4719-30BB-B02E-CCFC-0A64E7808E0D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="731520" y="5935980"/>
+          <a:ext cx="7597798" cy="1356478"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>434843</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>7856</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2D69C1B-73AE-61BD-C6D6-1CC4EFF359EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1333500" y="9723120"/>
+          <a:ext cx="5806943" cy="2720576"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>549573</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76302</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59B2E61A-5F83-913D-7F63-C2D8DED7CCD3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8069580" y="1752600"/>
+          <a:ext cx="10767993" cy="1181202"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>80887</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>167639</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>221553</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>61432</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A91853DA-667F-3BB9-D36E-4B4ED02081D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9834487" y="4488179"/>
+          <a:ext cx="3188666" cy="2636993"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>572131</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>7795</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{093BB147-6361-7047-7431-FC0B650E27FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="9075420"/>
+          <a:ext cx="7277731" cy="2019475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>31334</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>107002</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EAEC2AE-73F2-6E9C-CB36-ABF445298760}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8702040" y="13312994"/>
+          <a:ext cx="5417820" cy="2635988"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3243,8 +3773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B298CC97-231C-4C0A-8360-468EEE6A49D9}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3588,7 +4118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E5710C1-FC15-46B3-AB46-1AADB5C0B104}">
   <dimension ref="B3:AB175"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="U90" sqref="U90"/>
     </sheetView>
   </sheetViews>
@@ -3682,4 +4212,468 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DF5D23-439A-4B37-91E8-C097BD641D30}">
+  <dimension ref="B1:Q98"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:17" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="D1" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" s="14"/>
+      <c r="Q1" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M2" s="14"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="M3" s="14"/>
+      <c r="O3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="M5" s="14"/>
+      <c r="O5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M6" s="14"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="M7" s="14"/>
+      <c r="O7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M8" s="14"/>
+      <c r="O8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" s="14"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" s="14"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+      <c r="M11" s="14"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M12" s="14"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M13" s="14"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M14" s="14"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M15" s="14"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="M16" s="14"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M17" s="14"/>
+      <c r="O17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M18" s="14"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M19" s="14"/>
+      <c r="O19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M20" s="14"/>
+      <c r="P20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M21" s="14"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M22" s="14"/>
+      <c r="O22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M23" s="14"/>
+      <c r="O23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M24" s="14"/>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M25" s="14"/>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M26" s="14"/>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M27" s="14"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M28" s="14"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="E29" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="M29" s="14"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>90</v>
+      </c>
+      <c r="M30" s="14"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M31" s="14"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>96</v>
+      </c>
+      <c r="M32" s="14"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M33" s="14"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M34" s="14"/>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M35" s="14"/>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M36" s="14"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M37" s="14"/>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M38" s="14"/>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M39" s="14"/>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M40" s="14"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M41" s="14"/>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>91</v>
+      </c>
+      <c r="M42" s="14"/>
+      <c r="O42" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>95</v>
+      </c>
+      <c r="M43" s="14"/>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>97</v>
+      </c>
+      <c r="M44" s="14"/>
+      <c r="O44" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>92</v>
+      </c>
+      <c r="M45" s="14"/>
+      <c r="P45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>112</v>
+      </c>
+      <c r="M46" s="14"/>
+      <c r="P46" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>113</v>
+      </c>
+      <c r="M47" s="14"/>
+      <c r="P47" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>93</v>
+      </c>
+      <c r="M48" s="14"/>
+      <c r="P48" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>89</v>
+      </c>
+      <c r="M49" s="14"/>
+      <c r="P49" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>98</v>
+      </c>
+      <c r="M50" s="14"/>
+    </row>
+    <row r="51" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>99</v>
+      </c>
+      <c r="M51" s="14"/>
+    </row>
+    <row r="52" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>100</v>
+      </c>
+      <c r="M52" s="14"/>
+    </row>
+    <row r="53" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>102</v>
+      </c>
+      <c r="M53" s="14"/>
+    </row>
+    <row r="54" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="M54" s="14"/>
+    </row>
+    <row r="55" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="M55" s="14"/>
+    </row>
+    <row r="56" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="M56" s="14"/>
+    </row>
+    <row r="57" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="M57" s="14"/>
+    </row>
+    <row r="58" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="M58" s="14"/>
+    </row>
+    <row r="59" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="M59" s="14"/>
+    </row>
+    <row r="60" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="M60" s="14"/>
+    </row>
+    <row r="61" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="M61" s="14"/>
+    </row>
+    <row r="62" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="M62" s="14"/>
+      <c r="P62" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="M63" s="14"/>
+      <c r="P63" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="M64" s="14"/>
+      <c r="P64" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M65" s="14"/>
+      <c r="P65" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="66" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M66" s="14"/>
+      <c r="P66" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M67" s="14"/>
+      <c r="P67" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="68" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M68" s="14"/>
+      <c r="P68" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="69" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M69" s="14"/>
+      <c r="P69" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M70" s="14"/>
+      <c r="P70" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M71" s="14"/>
+    </row>
+    <row r="72" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M72" s="14"/>
+    </row>
+    <row r="73" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M73" s="14"/>
+    </row>
+    <row r="74" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M74" s="14"/>
+    </row>
+    <row r="75" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M75" s="14"/>
+    </row>
+    <row r="76" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M76" s="14"/>
+    </row>
+    <row r="77" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M77" s="14"/>
+    </row>
+    <row r="78" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M78" s="14"/>
+    </row>
+    <row r="79" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M79" s="14"/>
+    </row>
+    <row r="80" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M80" s="14"/>
+    </row>
+    <row r="81" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M81" s="14"/>
+    </row>
+    <row r="82" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M82" s="14"/>
+    </row>
+    <row r="83" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M83" s="14"/>
+    </row>
+    <row r="84" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M84" s="14"/>
+    </row>
+    <row r="85" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M85" s="14"/>
+    </row>
+    <row r="86" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M86" s="14"/>
+    </row>
+    <row r="87" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M87" s="14"/>
+    </row>
+    <row r="88" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M88" s="14"/>
+    </row>
+    <row r="89" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M89" s="14"/>
+      <c r="P89" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="90" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M90" s="14"/>
+      <c r="P90" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="91" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M91" s="14"/>
+    </row>
+    <row r="92" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M92" s="14"/>
+    </row>
+    <row r="93" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M93" s="14"/>
+    </row>
+    <row r="94" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M94" s="14"/>
+    </row>
+    <row r="95" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M95" s="14"/>
+    </row>
+    <row r="96" spans="13:16" x14ac:dyDescent="0.3">
+      <c r="M96" s="14"/>
+    </row>
+    <row r="97" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M97" s="14"/>
+    </row>
+    <row r="98" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M98" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>